<commit_message>
selenium gtranslate bug fixed
</commit_message>
<xml_diff>
--- a/____Selenium____/testRun2/Sheet-3.xlsx
+++ b/____Selenium____/testRun2/Sheet-3.xlsx
@@ -5,10 +5,10 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rober\Desktop\Scrapy\____Selenium____\testRun2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1436AC0-E773-4367-8696-707F2A8F14EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{069DF74A-5A1A-46F5-8590-E09B065EC0EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1515" yWindow="2115" windowWidth="21600" windowHeight="11385" xr2:uid="{A0C470EB-CFCF-4D8C-96D7-72A696661E05}"/>
   </bookViews>
@@ -20278,9 +20278,6 @@
     <t>Gbord koto valo.</t>
   </si>
   <si>
-    <t xml:space="preserve"> scrool kore 20/30 second er video pann nai???</t>
-  </si>
-  <si>
     <t xml:space="preserve"> o gula Torrent site e paben..</t>
   </si>
   <si>
@@ -20313,6 +20310,9 @@
   </si>
   <si>
     <t>apnar phone e maybe support korbe nah custom rom use kore dekhte paren</t>
+  </si>
+  <si>
+    <t>The aristrocrat hotel</t>
   </si>
 </sst>
 </file>
@@ -20740,8 +20740,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:A12188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20757,27 +20757,27 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>6695</v>
+        <v>6706</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>6696</v>
+        <v>6695</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>6697</v>
+        <v>6696</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>6698</v>
+        <v>6697</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>6705</v>
+        <v>6704</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
@@ -20787,37 +20787,37 @@
     </row>
     <row r="8" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6699</v>
+        <v>6698</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>6700</v>
+        <v>6699</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>6701</v>
+        <v>6700</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>6702</v>
+        <v>6701</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>6703</v>
+        <v>6702</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>6704</v>
+        <v>6703</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>6706</v>
+        <v>6705</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>